<commit_message>
Grade sheet updated with comments and scores for all four assignments
</commit_message>
<xml_diff>
--- a/Grades.xlsx
+++ b/Grades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BAIS\Fall 2019\GA\Big Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C1BC19-5C70-4A62-879A-E337EBC6A4FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FB3300-EDE7-4A63-94B9-5822B366A843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="56">
   <si>
     <t>Student</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Cassandra Java</t>
   </si>
   <si>
-    <t>Correct but incomplete. Did not show java class file or the jar file creation process</t>
-  </si>
-  <si>
     <t>Hive / Pig / Impala Assignment</t>
   </si>
   <si>
@@ -160,34 +157,40 @@
     <t>Complete and correct</t>
   </si>
   <si>
-    <t>Complete and correct. But the submission has no audio.</t>
-  </si>
-  <si>
     <t>Complete and correct (Explained the results from a previous session. Did not show the execution of any queries)</t>
   </si>
   <si>
-    <t>Complete and correct. Did not submit the video.</t>
-  </si>
-  <si>
     <t>Questions 3.2 and 3.4 are incomplete and are partially incorrect. Did not submit the code.</t>
   </si>
   <si>
     <t>Complete and correct. Did not submit the code.</t>
   </si>
   <si>
-    <t>Complete but the answers for questions 3.2 aand 3.4 are partially incorrect.</t>
-  </si>
-  <si>
-    <t>Complete but the answer for question 3.3 is partially incorrect</t>
-  </si>
-  <si>
     <t>Questions 3.2 and 3.4 are incomplete and are partially incorrect.</t>
   </si>
   <si>
     <t>Question 3.4's execution was not shown in the video. Question 3.2 was partiaally incorrect. Did not submit code. Video submission had no audio.</t>
   </si>
   <si>
-    <t>Correct and complete. But due to no audio in the submitted video, not able to listen to the explanation.</t>
+    <t>Correct but incomplete. Did not show java class file/jar file creation process</t>
+  </si>
+  <si>
+    <t>Submission has no audio</t>
+  </si>
+  <si>
+    <t>No Video submitted</t>
+  </si>
+  <si>
+    <t>Answers for questions 3.2 and 3.4 are partially incorrect.</t>
+  </si>
+  <si>
+    <t>Did not submit the code</t>
+  </si>
+  <si>
+    <t>Answer for question 3.3 is partially incorrect (Found least wins when the question is to find the most wins)</t>
+  </si>
+  <si>
+    <t>Submission has no audio.</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1206,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>37</v>
@@ -1445,7 +1448,7 @@
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="95" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1761,10 +1764,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1805,10 +1808,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,7 +1841,7 @@
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="132.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1846,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -1860,7 +1863,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,7 +1874,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1879,10 +1882,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1890,10 +1893,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,7 +1907,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,7 +1918,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,7 +1929,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,7 +1940,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,7 +1951,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,7 +1962,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,7 +1973,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,7 +1984,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,7 +1995,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2000,10 +2003,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,7 +2017,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,7 +2028,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2036,7 +2039,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2047,7 +2050,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2058,7 +2061,7 @@
         <v>9.5</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2069,7 +2072,7 @@
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2080,7 +2083,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2091,7 +2094,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2102,7 +2105,7 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2113,7 +2116,7 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2124,7 +2127,7 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2135,7 +2138,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,7 +2149,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,10 +2157,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2168,7 +2171,7 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2179,7 +2182,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,7 +2193,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,10 +2201,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2212,7 +2215,7 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
         <v>35</v>
@@ -2257,7 +2260,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2268,7 +2271,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2282,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2293,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2304,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2315,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2326,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2337,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2348,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2359,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2370,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,7 +2381,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,7 +2392,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2403,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2414,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2422,7 +2425,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,7 +2436,7 @@
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2444,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2455,7 +2458,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,7 +2469,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2480,7 @@
         <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2491,7 @@
         <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,7 +2502,7 @@
         <v>10</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,7 +2513,7 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,7 +2524,7 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2532,7 +2535,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,7 +2546,7 @@
         <v>10</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,7 +2557,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,7 +2568,7 @@
         <v>10</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,7 +2579,7 @@
         <v>10</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,7 +2590,7 @@
         <v>10</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -2595,10 +2598,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -2609,7 +2612,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>